<commit_message>
Updated the stats in the excel file
</commit_message>
<xml_diff>
--- a/ExcelFile.xlsx
+++ b/ExcelFile.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ymulonda/Documents/Demo/Group-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Jeevan\Official\Masters Program St. Thomas\DataScience\Courses\06. Spring. 2021\SEIS_763\763_ML_Group_Project\group-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB4811FA-3BF7-3747-B575-81292CDBE767}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D1DA73-2AFD-4B58-88CA-D4011787FFF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{706537C4-E01E-8A49-AA1E-E4A11AD36849}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{706537C4-E01E-8A49-AA1E-E4A11AD36849}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
   <si>
     <t>Lasso</t>
   </si>
@@ -42,18 +48,33 @@
     <t>SVM</t>
   </si>
   <si>
-    <t>linear</t>
-  </si>
-  <si>
-    <t>One Class SVM</t>
-  </si>
-  <si>
-    <t>weightedLogisticRegression</t>
+    <t>One Class (Stroke) SVM</t>
+  </si>
+  <si>
+    <t>One Class (Not Stroke) SVM</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Weighted Logistic Regression</t>
+  </si>
+  <si>
+    <t>Voting Classifier - Hard Voting</t>
+  </si>
+  <si>
+    <t>Voting Classifier - Soft Voting</t>
+  </si>
+  <si>
+    <t>Gaussian NB</t>
   </si>
   <si>
     <t>RMSE</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
@@ -67,30 +88,6 @@
   </si>
   <si>
     <t>AUC</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Column2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -126,17 +123,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -168,15 +188,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A029714D-46E6-DB46-9D9F-E6784022AF0E}" name="Table2" displayName="Table2" ref="A1:F9" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:F9" xr:uid="{F0562D24-337B-AD44-A090-F349E081D17D}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C6D05FFB-2658-5D4C-B732-414EA28996C7}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{B1C667FD-3219-7542-A4C3-83DBAF6E2D1E}" name="Column2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{0ED3223D-E0BB-CD4D-9240-41561DADA9CA}" name="Column3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{41609E91-5DA7-3547-A8D9-1988F59B3130}" name="Column4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{3F0D8968-93F8-1241-8696-270A45172581}" name="Column5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{245460AB-CA4E-144C-95B8-03E74FD09406}" name="Column6" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A029714D-46E6-DB46-9D9F-E6784022AF0E}" name="Table2" displayName="Table2" ref="A1:K7" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:K7" xr:uid="{F0562D24-337B-AD44-A090-F349E081D17D}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{C6D05FFB-2658-5D4C-B732-414EA28996C7}" name="Metrics"/>
+    <tableColumn id="2" xr3:uid="{B1C667FD-3219-7542-A4C3-83DBAF6E2D1E}" name="linear" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{0ED3223D-E0BB-CD4D-9240-41561DADA9CA}" name="Lasso" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{41609E91-5DA7-3547-A8D9-1988F59B3130}" name="SVM" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{3F0D8968-93F8-1241-8696-270A45172581}" name="One Class (Stroke) SVM" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{F99755EC-1E66-4BB3-B203-08A1255B8213}" name="One Class (Not Stroke) SVM" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{48F00E57-0D04-4F8B-A0A1-E868F355AA9C}" name="Logistic Regression" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{245460AB-CA4E-144C-95B8-03E74FD09406}" name="Weighted Logistic Regression" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{6C58440E-35F2-44DB-9FFB-390FDE3D6AE2}" name="Voting Classifier - Hard Voting" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{2D33AD24-CBD2-44E0-A632-DF17BE03E3DA}" name="Voting Classifier - Soft Voting" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{D04358EA-99B0-4824-9495-3F8D1C43EFD0}" name="Gaussian NB" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -479,174 +504,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4570A7-0D52-E148-A921-A8650002DCDE}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1"/>
+    <col min="3" max="4" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="39.375" customWidth="1"/>
+    <col min="10" max="10" width="34.125" customWidth="1"/>
+    <col min="11" max="11" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="2">
+        <v>0.21078648433692301</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.55119510789441095</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.52061231448755196</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.71330656959747596</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.226649206955812</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.712963551270549</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.53680580256487398</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.46868680265438101</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.89683068845648795</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>9.63761901567598E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-5.1789240025702403</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-4.5122768074459101</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-9.3479564616313198</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-4.4745604299316399E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-9.3380065034951407</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-4.86052534221235</v>
+      </c>
+      <c r="J3" s="2">
+        <v>-3.4675312031466001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-15.3577311758864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.69618395303326797</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.72896281800391305</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.49119373776907999</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.94863013698630105</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.48630136986301298</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.71183953033268099</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.780332681017612</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.19569471624266099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.63207547169811296</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.48113207547169801</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.20754716981131999</v>
+      </c>
+      <c r="G5" s="2">
+        <v>9.4339622641509396E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.98113207547169801</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.64150943396226401</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.79245283018867896</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.98113207547169801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.103235747303543</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9.27272727272727E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.24948875255623E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>9.0277777777777707E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.109854604200323</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.164383561643835</v>
+      </c>
+      <c r="K6" s="2">
+        <v>5.9564719358533698E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.21078648433692301</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.55119510789441095</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.52061231448755196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.63761901567598E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>-5.1789240025702403</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-4.5122768074459101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.69618395303326797</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.72896281800391305</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.94814090019569397</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.63207547169811296</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.48113207547169801</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.103235747303543</v>
-      </c>
-      <c r="E8" s="1">
-        <v>9.27272727272727E-2</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.5</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.66588293708744595</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.611825067663609</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.35712755807387497</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.50471698113207497</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.72302217808672598</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.67859785423603403</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.78606129641528899</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.56693342679673597</v>
       </c>
     </row>
   </sheetData>
@@ -655,4 +775,186 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035652743EA779E4EA7F50F9CC6733EF7" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d18c07f4830c91a57ecb11d6b6c3ad6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="359a6c4c-802d-4fb0-90f7-076d253ee700" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae2d2492f90fa89cd4a467ba5e11106f" ns2:_="">
+    <xsd:import namespace="359a6c4c-802d-4fb0-90f7-076d253ee700"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="359a6c4c-802d-4fb0-90f7-076d253ee700" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55704C74-CF27-4C46-86C3-D575AC6677FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4805FB7B-6F7B-4E02-B2E7-368705152653}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{860AB4DF-4547-4C0F-BF42-85B2520D5E70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="359a6c4c-802d-4fb0-90f7-076d253ee700"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>